<commit_message>
content/images for ATC taping
</commit_message>
<xml_diff>
--- a/status/RC1_punchlist_v3.xlsx
+++ b/status/RC1_punchlist_v3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="1680" windowWidth="23200" windowHeight="17340" tabRatio="500"/>
+    <workbookView xWindow="260" yWindow="0" windowWidth="23200" windowHeight="17340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>add Tru-Medical logomark to pages</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -29,35 +29,19 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Make Sombra in Dual location, add to Topical Analgesics under Clinic Supplies</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Consolidate Formfit Wrist Brace in Orthopedics/Hand &amp; Wrist 750103- (8”) &amp; 750104- (6”) together. Put additional bullet to read Offered in both 6” and 8” models</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Place Sling (currently in Collars &amp; Slings) also in Shoulder as well</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Consolidate Stainless Steel Goniometers in Eval section</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Take out NPWT Canister &amp; NPWT Non-Canister from Wound Care</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>TruMedical —&gt; About TruMedical in menu</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>color of footer:  gray-&gt;black</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">vertical band of white to the right </t>
+    <t>changed</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>changed</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">— product images used on leaf-level category pages for Taping &amp; Wrapping/Wrapping are too large. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>— 'large' images used on product pages are squished to 72px; should be 250px high; width open as long as inside 700px.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -65,7 +49,7 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">Under Modalities, Continuous Passive Motion pic is wrong; Mandy sent the right pic </t>
+    <t>Hypoallergeic 'Pape' -&gt; 'Tape'</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -74,6 +58,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="10"/>
         <color indexed="12"/>
         <rFont val="Verdana"/>
@@ -82,6 +67,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="10"/>
         <rFont val="Verdana"/>
       </rPr>
@@ -90,6 +76,58 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>stretched/squished/too large</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>pictures</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>categorization/consolidation</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>other</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Make Sombra in Dual location, add to Topical Analgesics under Clinic Supplies</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Consolidate Formfit Wrist Brace in Orthopedics/Hand &amp; Wrist 750103- (8”) &amp; 750104- (6”) together. Put additional bullet to read Offered in both 6” and 8” models</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Place Sling (currently in Collars &amp; Slings) also in Shoulder as well</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Consolidate Stainless Steel Goniometers in Eval section</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Take out NPWT Canister &amp; NPWT Non-Canister from Wound Care</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>TruMedical —&gt; About TruMedical in menu</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>color of footer:  gray-&gt;black</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">vertical band of white to the right </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Under Modalities, Continuous Passive Motion pic is wrong; Mandy sent the right pic </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>Need icons for LTL trucking, no-latex, etc; using stand-ins now</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -141,23 +179,7 @@
     <t>Gameplan for Promotion area and Tru Family of Products Buttons?</t>
   </si>
   <si>
-    <t>pictures</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>other</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>ui/layout related</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>categorization/consolidation</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stretched/squished/too large</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -210,7 +232,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -250,6 +272,11 @@
       <color indexed="57"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="17"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -271,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -285,6 +312,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -631,26 +659,26 @@
   <sheetData>
     <row r="1" spans="1:7" ht="26">
       <c r="A1" s="3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -661,7 +689,7 @@
         <v>39536</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="8"/>
@@ -669,7 +697,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -680,7 +708,7 @@
         <v>39536</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="8"/>
@@ -689,7 +717,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -705,7 +733,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -734,7 +762,7 @@
         <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -746,7 +774,7 @@
         <v>6</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -758,7 +786,7 @@
         <v>7</v>
       </c>
       <c r="G10" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -770,7 +798,7 @@
         <v>8</v>
       </c>
       <c r="G11" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -779,19 +807,19 @@
     <row r="13" spans="1:7">
       <c r="A13" s="2"/>
       <c r="D13" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2"/>
-      <c r="E14" t="s">
-        <v>26</v>
+      <c r="E14" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2"/>
-      <c r="F15" t="s">
-        <v>12</v>
+      <c r="F15" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -803,7 +831,7 @@
         <v>9</v>
       </c>
       <c r="G16" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -815,7 +843,7 @@
         <v>10</v>
       </c>
       <c r="G17" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -827,7 +855,7 @@
         <v>11</v>
       </c>
       <c r="G18" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -839,7 +867,7 @@
         <v>12</v>
       </c>
       <c r="G19" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -851,7 +879,7 @@
         <v>13</v>
       </c>
       <c r="G20" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -863,71 +891,74 @@
         <v>14</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="2"/>
-      <c r="F22" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="2">
-        <v>39536</v>
-      </c>
-      <c r="F23">
+      <c r="F22" s="10">
         <f>F21+1</f>
         <v>15</v>
       </c>
-      <c r="G23" t="s">
-        <v>22</v>
+      <c r="G22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="2"/>
+      <c r="F23" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="2">
         <v>39536</v>
       </c>
-      <c r="F24">
-        <f>F23+1</f>
+      <c r="G24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="2"/>
+      <c r="B25" s="7">
+        <v>39537</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11">
+        <f>F22+1</f>
         <v>16</v>
       </c>
-      <c r="G24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="2">
-        <v>39536</v>
-      </c>
-      <c r="F25">
-        <f>F24+1</f>
+      <c r="G25" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2">
+        <v>39537</v>
+      </c>
+      <c r="F26">
+        <f>F25+1</f>
         <v>17</v>
       </c>
-      <c r="G25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="5">
-        <v>39537</v>
-      </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4">
-        <f>F25+1</f>
+      <c r="G26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="2">
+        <v>39536</v>
+      </c>
+      <c r="F27">
+        <f>F26+1</f>
         <v>18</v>
       </c>
-      <c r="G26" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="2"/>
-      <c r="E27" t="s">
-        <v>31</v>
+      <c r="G27" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -935,29 +966,33 @@
         <v>39536</v>
       </c>
       <c r="F28">
-        <f>F26+1</f>
+        <f>F27+1</f>
         <v>19</v>
       </c>
       <c r="G28" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="2"/>
-      <c r="E29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="2">
-        <v>39536</v>
-      </c>
-      <c r="F30">
+      <c r="A29" s="5">
+        <v>39537</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4">
         <f>F28+1</f>
         <v>20</v>
       </c>
-      <c r="G30" t="s">
-        <v>2</v>
+      <c r="G29" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="2"/>
+      <c r="E30" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -965,35 +1000,27 @@
         <v>39536</v>
       </c>
       <c r="F31">
-        <f>F30+1</f>
+        <f>F29+1</f>
         <v>21</v>
       </c>
       <c r="G31" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="2">
-        <v>39536</v>
-      </c>
+      <c r="A32" s="2"/>
       <c r="F32">
-        <f t="shared" ref="F32:F35" si="2">F31+1</f>
+        <f>F31+1</f>
         <v>22</v>
       </c>
       <c r="G32" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="2">
-        <v>39536</v>
-      </c>
-      <c r="F33">
-        <f t="shared" si="2"/>
-        <v>23</v>
-      </c>
-      <c r="G33" t="s">
-        <v>5</v>
+      <c r="A33" s="2"/>
+      <c r="E33" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1001,11 +1028,11 @@
         <v>39536</v>
       </c>
       <c r="F34">
-        <f t="shared" si="2"/>
-        <v>24</v>
+        <f>F32+1</f>
+        <v>23</v>
       </c>
       <c r="G34" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1013,17 +1040,23 @@
         <v>39536</v>
       </c>
       <c r="F35">
-        <f t="shared" si="2"/>
+        <f>F34+1</f>
+        <v>24</v>
+      </c>
+      <c r="G35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="2">
+        <v>39536</v>
+      </c>
+      <c r="F36">
+        <f t="shared" ref="F36:F37" si="2">F35+1</f>
         <v>25</v>
       </c>
-      <c r="G35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="2"/>
-      <c r="E36" t="s">
-        <v>27</v>
+      <c r="G36" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1031,20 +1064,29 @@
         <v>39536</v>
       </c>
       <c r="F37">
-        <f>F35+1</f>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="G37" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="2"/>
+      <c r="A38" s="2">
+        <v>39536</v>
+      </c>
+      <c r="F38">
+        <f>F37+1</f>
+        <v>27</v>
+      </c>
+      <c r="G38" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="2"/>
-      <c r="D39" s="1" t="s">
-        <v>33</v>
+      <c r="E39" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1052,23 +1094,44 @@
         <v>39536</v>
       </c>
       <c r="F40">
-        <f>F37+1</f>
-        <v>27</v>
+        <f>F38+1</f>
+        <v>28</v>
       </c>
       <c r="G40" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="2">
-        <v>39536</v>
-      </c>
-      <c r="F41">
+      <c r="A41" s="2"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="2"/>
+      <c r="D42" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="2">
+        <v>39536</v>
+      </c>
+      <c r="F43">
         <f>F40+1</f>
-        <v>28</v>
-      </c>
-      <c r="G41" t="s">
-        <v>25</v>
+        <v>29</v>
+      </c>
+      <c r="G43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="2">
+        <v>39536</v>
+      </c>
+      <c r="F44">
+        <f>F43+1</f>
+        <v>30</v>
+      </c>
+      <c r="G44" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>